<commit_message>
11.8.18 plots and analysis
</commit_message>
<xml_diff>
--- a/Article Coding/Count - Logistic Article Coding Sheet_Max.xlsx
+++ b/Article Coding/Count - Logistic Article Coding Sheet_Max.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="9168"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="53">
   <si>
     <t>Result #</t>
   </si>
@@ -116,9 +116,6 @@
     <t>Coefficient figure</t>
   </si>
   <si>
-    <t>Report transformed OR/RR</t>
-  </si>
-  <si>
     <t>Outcome type</t>
   </si>
   <si>
@@ -161,9 +158,6 @@
     <t>Figure shows predicted counts, but not described in text</t>
   </si>
   <si>
-    <t>Figure shows predicted probs, but not descirbed in text</t>
-  </si>
-  <si>
     <t>JAbP</t>
   </si>
   <si>
@@ -180,6 +174,15 @@
   </si>
   <si>
     <t>Used GEE; figure shows predicted counts, not described in text</t>
+  </si>
+  <si>
+    <t>Report transformed coefficient? (OR/RR)</t>
+  </si>
+  <si>
+    <t>Figure shows predicted probs, but not described in text</t>
+  </si>
+  <si>
+    <t>This is David Atkins' tutorial paper</t>
   </si>
 </sst>
 </file>
@@ -565,7 +568,7 @@
   <dimension ref="A2:Q58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -585,7 +588,7 @@
       </c>
       <c r="C2" s="2">
         <f>COUNTIF(C4:C60,"Y")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E2" s="4">
         <f>COUNTIF(E4:E58,"Yes")/COUNTIF($C4:$C58,"Y")</f>
@@ -619,13 +622,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>29</v>
@@ -634,26 +637,26 @@
         <v>1</v>
       </c>
       <c r="H3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="K3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L3" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="O3" s="3">
         <f>COUNTIF(D:D,P3)/COUNTIF($C4:$C58,"Y")</f>
-        <v>0.2</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="P3" t="s">
         <v>2</v>
@@ -664,47 +667,47 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L4" s="2">
         <v>202</v>
       </c>
       <c r="M4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O4" s="3">
         <f t="shared" ref="O4:O11" si="0">COUNTIF(D:D,P4)/COUNTIF($C5:$C59,"Y")</f>
-        <v>0.25</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="P4" t="s">
         <v>5</v>
@@ -715,47 +718,47 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L5" s="2">
         <v>84</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O5" s="3">
         <f t="shared" si="0"/>
-        <v>0.66666666666666663</v>
+        <v>0.8</v>
       </c>
       <c r="P5" t="s">
         <v>8</v>
@@ -766,37 +769,37 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L6" s="2">
         <v>623</v>
@@ -814,47 +817,47 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L7" s="2">
         <v>722</v>
       </c>
       <c r="M7" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="O7" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="P7" t="s">
         <v>13</v>
@@ -865,43 +868,43 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B8">
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O8" s="3">
         <f t="shared" si="0"/>
@@ -916,44 +919,47 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B9">
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L9" s="2">
         <v>143</v>
       </c>
       <c r="M9" t="s">
-        <v>51</v>
-      </c>
-      <c r="O9" s="3" t="e">
+        <v>49</v>
+      </c>
+      <c r="O9" s="3">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P9" t="s">
         <v>22</v>
@@ -963,12 +969,45 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
       <c r="B10">
         <v>7</v>
       </c>
-      <c r="O10" s="3" t="e">
+      <c r="C10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L10" s="2">
+        <v>195</v>
+      </c>
+      <c r="O10" s="3">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P10" t="s">
         <v>24</v>
@@ -978,8 +1017,41 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
       <c r="B11">
         <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11" s="2">
+        <v>307</v>
       </c>
       <c r="O11" s="3" t="e">
         <f t="shared" si="0"/>
@@ -995,6 +1067,39 @@
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>9</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
writing progress and coing updates
</commit_message>
<xml_diff>
--- a/Article Coding/Count - Logistic Article Coding Sheet_Max.xlsx
+++ b/Article Coding/Count - Logistic Article Coding Sheet_Max.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="58">
   <si>
     <t>Result #</t>
   </si>
@@ -183,6 +183,21 @@
   </si>
   <si>
     <t>This is David Atkins' tutorial paper</t>
+  </si>
+  <si>
+    <t>This is a correction to David Atkins' tutorial paper</t>
+  </si>
+  <si>
+    <t>Linear Regression</t>
+  </si>
+  <si>
+    <t>A series of univariate LR's, no multivariate model</t>
+  </si>
+  <si>
+    <t>IRT</t>
+  </si>
+  <si>
+    <t>IRT paper</t>
   </si>
 </sst>
 </file>
@@ -568,7 +583,7 @@
   <dimension ref="A2:Q58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -588,7 +603,7 @@
       </c>
       <c r="C2" s="2">
         <f>COUNTIF(C4:C60,"Y")</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E2" s="4">
         <f>COUNTIF(E4:E58,"Yes")/COUNTIF($C4:$C58,"Y")</f>
@@ -656,7 +671,7 @@
       </c>
       <c r="O3" s="3">
         <f>COUNTIF(D:D,P3)/COUNTIF($C4:$C58,"Y")</f>
-        <v>0.14285714285714285</v>
+        <v>0.1</v>
       </c>
       <c r="P3" t="s">
         <v>2</v>
@@ -707,7 +722,7 @@
       </c>
       <c r="O4" s="3">
         <f t="shared" ref="O4:O11" si="0">COUNTIF(D:D,P4)/COUNTIF($C5:$C59,"Y")</f>
-        <v>0.16666666666666666</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="P4" t="s">
         <v>5</v>
@@ -758,7 +773,7 @@
       </c>
       <c r="O5" s="3">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>0.875</v>
       </c>
       <c r="P5" t="s">
         <v>8</v>
@@ -857,7 +872,7 @@
       </c>
       <c r="O7" s="3">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="P7" t="s">
         <v>13</v>
@@ -1053,9 +1068,9 @@
       <c r="L11" s="2">
         <v>307</v>
       </c>
-      <c r="O11" s="3" t="e">
+      <c r="O11" s="3">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="P11" t="s">
         <v>26</v>
@@ -1106,110 +1121,353 @@
       <c r="B13">
         <v>10</v>
       </c>
+      <c r="C13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M13" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>11</v>
       </c>
+      <c r="C14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M14" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
       <c r="B15">
         <v>12</v>
       </c>
+      <c r="C15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L15" s="2">
+        <v>70</v>
+      </c>
+      <c r="M15" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
       <c r="B16">
         <v>13</v>
       </c>
+      <c r="C16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L16" s="2">
+        <v>2451</v>
+      </c>
+      <c r="M16" t="s">
+        <v>55</v>
+      </c>
       <c r="P16" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
       <c r="B17">
         <v>14</v>
       </c>
+      <c r="C17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M17" t="s">
+        <v>46</v>
+      </c>
       <c r="P17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
       <c r="B18">
         <v>15</v>
       </c>
+      <c r="C18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L18" s="2">
+        <v>399</v>
+      </c>
       <c r="P18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
       <c r="B19">
         <v>16</v>
       </c>
+      <c r="C19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M19" t="s">
+        <v>57</v>
+      </c>
       <c r="P19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
coding sheet update and minutes
</commit_message>
<xml_diff>
--- a/Article Coding/Count - Logistic Article Coding Sheet_Max.xlsx
+++ b/Article Coding/Count - Logistic Article Coding Sheet_Max.xlsx
@@ -971,9 +971,9 @@
   <dimension ref="A2:R58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomLeft" activeCell="M3" sqref="M1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>